<commit_message>
Commentaires sur la fiche de temps
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine2.xlsx
+++ b/FichesTemps/LouisGarceauSemaine2.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7977B7BE-8E56-415E-848F-7802C5212ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77ED756-28D2-48A8-83CE-061BD2D95699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="948" windowWidth="15960" windowHeight="9960" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="948" windowWidth="15960" windowHeight="9960" tabRatio="768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temps" sheetId="15" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="107">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -452,6 +452,21 @@
   </si>
   <si>
     <t>19, 21</t>
+  </si>
+  <si>
+    <t>Je pense que j'ai bien travaillé et que j'ai appris avec la technologie React Native. Cependant, j'ai un peu moins participé pour la planification de début de semaine.</t>
+  </si>
+  <si>
+    <t>Jean-Philippe a très bien travaillé. Il a été très important dans le développement de l'application et dans les rencontres pour planifier.</t>
+  </si>
+  <si>
+    <t>Victor a beaucoup avancé le projet, mais à certains moments, il ne se gêne pas pour dire son opinion.</t>
+  </si>
+  <si>
+    <t>Maxime a bien développé l'application, mais il a été un peu moins présent pour parler en ligne. Ça n'a vraiment pas trop affecté négativement le travail sur le projet.</t>
+  </si>
+  <si>
+    <t>Karl a travaillé bien pour développer l'application, mais lui-même admet qu'il a passé trop de temps sur des fonctionnalités qui auraient dû être faites plus rapidement.</t>
   </si>
 </sst>
 </file>
@@ -958,6 +973,10 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1070,10 +1089,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1834,7 +1849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1856,17 +1871,17 @@
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1883,40 +1898,40 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="31" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="32" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="34" t="str">
         <f>_xlfn.CONCAT("Évaluateur = ",Évaluateur!F14," ",Évaluateur!D30,CHAR(10),'Coéquipier 1'!D9:I9," ",'Coéquipier 1'!D10:I10," = ",'Coéquipier 1'!F11:I25," ",'Coéquipier 1'!D27:I27,CHAR(10),'Coéquipier 2'!D9:I9," ",'Coéquipier 2'!D10:I10," = ",'Coéquipier 2'!F11:I25,CHAR(10),'Coéquipier 3'!D9:I9," ",'Coéquipier 3'!D10:I10," = ",'Coéquipier 3'!F11:I25,CHAR(10),'Coéquipier 4'!D9:I9," ",'Coéquipier 4'!D10:I10," = ",'Coéquipier 4'!F11:I25,CHAR(10),'Coéquipier 5'!D9:I9," ",'Coéquipier 5'!D10:I10," = ",'Coéquipier 5'!F11:I25)</f>
-        <v>Évaluateur = 75 
-Jean-Philippe Belval = 75 
-Victor Turgeon = 75
-Karl Mainville = 75
-Maxime Aubin = 75
+        <v>Évaluateur = 72 Je pense que j'ai bien travaillé et que j'ai appris avec la technologie React Native. Cependant, j'ai un peu moins participé pour la planification de début de semaine.
+Jean-Philippe Belval = 74 Jean-Philippe a très bien travaillé. Il a été très important dans le développement de l'application et dans les rencontres pour planifier.
+Victor Turgeon = 73
+Karl Mainville = 72
+Maxime Aubin = 73
 Coéquipier 5 = à évaluer</v>
       </c>
       <c r="E8" s="10"/>
@@ -2045,7 +2060,7 @@
       <c r="A19" s="45">
         <v>44957</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="48" t="s">
         <v>99</v>
       </c>
       <c r="C19" s="47">
@@ -2077,7 +2092,7 @@
       <c r="A22" s="45">
         <v>44958</v>
       </c>
-      <c r="B22" s="84" t="s">
+      <c r="B22" s="48" t="s">
         <v>101</v>
       </c>
       <c r="C22" s="47">
@@ -2091,7 +2106,7 @@
       <c r="A23" s="45">
         <v>44958</v>
       </c>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="48" t="s">
         <v>100</v>
       </c>
       <c r="C23" s="47">
@@ -4856,7 +4871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D30" sqref="D30:I30"/>
     </sheetView>
   </sheetViews>
@@ -4883,26 +4898,26 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="8"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
       <c r="J3" s="10"/>
     </row>
@@ -4929,15 +4944,15 @@
       <c r="B6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4978,14 +4993,14 @@
       <c r="C10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" s="8" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5002,36 +5017,36 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
-      <c r="B12" s="54"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="61" t="str">
+      <c r="D12" s="62" t="str">
         <f>Temps!D6</f>
         <v>Louis</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
-      <c r="B13" s="54"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="61" t="str">
+      <c r="D13" s="62" t="str">
         <f>Temps!D7</f>
         <v>Garceau</v>
       </c>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -5047,13 +5062,13 @@
         <f>VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="64">
         <f>IFERROR(SUM(E14:E28),"Autoévaluation à faire")</f>
-        <v>75</v>
-      </c>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="65"/>
+        <v>72</v>
+      </c>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="66"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -5069,10 +5084,10 @@
         <f>VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="68"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="69"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -5088,10 +5103,10 @@
         <f>VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F16" s="66"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="68"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -5101,16 +5116,16 @@
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="12">
         <f>VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F17" s="66"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="68"/>
+        <v>4</v>
+      </c>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -5120,16 +5135,16 @@
         <v>12</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" s="12">
         <f>VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F18" s="66"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="68"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="69"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -5139,16 +5154,16 @@
         <v>13</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="12">
         <f>VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F19" s="66"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="68"/>
+        <v>4</v>
+      </c>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="69"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -5164,10 +5179,10 @@
         <f>VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F20" s="66"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="68"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="69"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -5183,10 +5198,10 @@
         <f>VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F21" s="66"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="68"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="69"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -5202,10 +5217,10 @@
         <f>VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F22" s="66"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="68"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="69"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -5221,10 +5236,10 @@
         <f>VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F23" s="66"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="68"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -5240,10 +5255,10 @@
         <f>VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="66"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="68"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="69"/>
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -5259,10 +5274,10 @@
         <f>VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="66"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="68"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="69"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -5278,10 +5293,10 @@
         <f>VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F26" s="66"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="68"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="69"/>
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -5297,10 +5312,10 @@
         <f>VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F27" s="66"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="68"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="69"/>
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5316,10 +5331,10 @@
         <f>VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F28" s="69"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="71"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5334,12 +5349,14 @@
       <c r="C30" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="58"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="60"/>
+      <c r="D30" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="61"/>
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -5450,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5477,26 +5494,26 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="8"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
       <c r="J3" s="10"/>
     </row>
@@ -5532,14 +5549,14 @@
       <c r="C7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5554,14 +5571,14 @@
       <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5570,14 +5587,14 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5593,13 +5610,13 @@
         <f>VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="74">
+      <c r="F11" s="75">
         <f>IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>75</v>
-      </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="76"/>
+        <v>74</v>
+      </c>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5615,10 +5632,10 @@
         <f>VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5634,10 +5651,10 @@
         <f>VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F13" s="77"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="80"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5653,10 +5670,10 @@
         <f>VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5672,10 +5689,10 @@
         <f>VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="80"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5691,10 +5708,10 @@
         <f>VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="80"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5710,10 +5727,10 @@
         <f>VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5729,10 +5746,10 @@
         <f>VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F18" s="77"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5748,10 +5765,10 @@
         <f>VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F19" s="77"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5761,16 +5778,16 @@
         <v>40</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="12">
         <f>VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F20" s="77"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5786,10 +5803,10 @@
         <f>VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="79"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5805,10 +5822,10 @@
         <f>VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5824,10 +5841,10 @@
         <f>VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F23" s="77"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="79"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="80"/>
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5843,10 +5860,10 @@
         <f>VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="77"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="79"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5862,10 +5879,10 @@
         <f>VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="83"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5880,12 +5897,14 @@
       <c r="C27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
+      <c r="D27" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -5994,7 +6013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:I27"/>
     </sheetView>
   </sheetViews>
@@ -6021,26 +6040,26 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="8"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
       <c r="J3" s="10"/>
     </row>
@@ -6076,14 +6095,14 @@
       <c r="C7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -6098,14 +6117,14 @@
       <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6114,14 +6133,14 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6137,13 +6156,13 @@
         <f>VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="74">
+      <c r="F11" s="75">
         <f>IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>75</v>
-      </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="76"/>
+        <v>73</v>
+      </c>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6159,10 +6178,10 @@
         <f>VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6178,10 +6197,10 @@
         <f>VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F13" s="77"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="80"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6197,10 +6216,10 @@
         <f>VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6216,10 +6235,10 @@
         <f>VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="80"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6235,10 +6254,10 @@
         <f>VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="80"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6248,16 +6267,16 @@
         <v>37</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="12">
         <f>VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6273,10 +6292,10 @@
         <f>VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F18" s="77"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6286,16 +6305,16 @@
         <v>39</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="12">
         <f>VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F19" s="77"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6311,10 +6330,10 @@
         <f>VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F20" s="77"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="79"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6330,10 +6349,10 @@
         <f>VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="79"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6349,10 +6368,10 @@
         <f>VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6368,10 +6387,10 @@
         <f>VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F23" s="77"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="79"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="80"/>
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6387,10 +6406,10 @@
         <f>VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="77"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="79"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6406,10 +6425,10 @@
         <f>VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="83"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6421,15 +6440,15 @@
     <row r="27" spans="1:10" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -6538,7 +6557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:I27"/>
     </sheetView>
   </sheetViews>
@@ -6565,26 +6584,26 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="8"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
       <c r="J3" s="10"/>
     </row>
@@ -6620,14 +6639,14 @@
       <c r="C7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -6642,14 +6661,14 @@
       <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6658,14 +6677,14 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6681,13 +6700,13 @@
         <f>VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="74">
+      <c r="F11" s="75">
         <f>IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>75</v>
-      </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="76"/>
+        <v>72</v>
+      </c>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6703,10 +6722,10 @@
         <f>VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6722,10 +6741,10 @@
         <f>VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F13" s="77"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="80"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6741,10 +6760,10 @@
         <f>VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6760,10 +6779,10 @@
         <f>VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="80"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6779,10 +6798,10 @@
         <f>VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="80"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6798,10 +6817,10 @@
         <f>VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6817,10 +6836,10 @@
         <f>VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F18" s="77"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6830,16 +6849,16 @@
         <v>39</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="12">
         <f>VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F19" s="77"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6855,10 +6874,10 @@
         <f>VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F20" s="77"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="79"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6874,10 +6893,10 @@
         <f>VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="79"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6887,16 +6906,16 @@
         <v>42</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="12">
         <f>VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F22" s="78"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6912,10 +6931,10 @@
         <f>VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F23" s="77"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="79"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="80"/>
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6925,16 +6944,16 @@
         <v>44</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="12">
         <f>VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F24" s="77"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F24" s="78"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6950,10 +6969,10 @@
         <f>VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="83"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6968,12 +6987,14 @@
       <c r="C27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
+      <c r="D27" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -7082,7 +7103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:I27"/>
     </sheetView>
   </sheetViews>
@@ -7109,26 +7130,26 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="8"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
       <c r="J3" s="10"/>
     </row>
@@ -7164,14 +7185,14 @@
       <c r="C7" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -7186,14 +7207,14 @@
       <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7202,14 +7223,14 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7225,13 +7246,13 @@
         <f>VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="74">
+      <c r="F11" s="75">
         <f>IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>75</v>
-      </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="76"/>
+        <v>73</v>
+      </c>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7247,10 +7268,10 @@
         <f>VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7266,10 +7287,10 @@
         <f>VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F13" s="77"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="80"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7285,10 +7306,10 @@
         <f>VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7304,10 +7325,10 @@
         <f>VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="80"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7317,16 +7338,16 @@
         <v>36</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="12">
         <f>VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="80"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7342,10 +7363,10 @@
         <f>VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7361,10 +7382,10 @@
         <f>VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F18" s="77"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7374,16 +7395,16 @@
         <v>39</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="12">
         <f>VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>5</v>
-      </c>
-      <c r="F19" s="77"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
+        <v>4</v>
+      </c>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7399,10 +7420,10 @@
         <f>VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F20" s="77"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="79"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7418,10 +7439,10 @@
         <f>VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="79"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7437,10 +7458,10 @@
         <f>VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7456,10 +7477,10 @@
         <f>VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F23" s="77"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="79"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="80"/>
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7475,10 +7496,10 @@
         <f>VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="77"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="79"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7494,10 +7515,10 @@
         <f>VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="83"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7512,12 +7533,14 @@
       <c r="C27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
+      <c r="D27" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -7653,26 +7676,26 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="8"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
       <c r="J3" s="10"/>
     </row>
@@ -7708,14 +7731,14 @@
       <c r="C7" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -7730,14 +7753,14 @@
       <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7746,14 +7769,14 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D10" s="73">
         <v>5</v>
       </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7767,13 +7790,13 @@
         <f>VLOOKUP('Coéquipier 5'!D11,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F11" s="74" t="str">
+      <c r="F11" s="75" t="str">
         <f>IFERROR(SUM(E11:E25),"à évaluer")</f>
         <v>à évaluer</v>
       </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7787,10 +7810,10 @@
         <f>VLOOKUP('Coéquipier 5'!D12,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7804,10 +7827,10 @@
         <f>VLOOKUP('Coéquipier 5'!D13,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F13" s="77"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="80"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7821,10 +7844,10 @@
         <f>VLOOKUP('Coéquipier 5'!D14,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7838,10 +7861,10 @@
         <f>VLOOKUP('Coéquipier 5'!D15,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="80"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7855,10 +7878,10 @@
         <f>VLOOKUP('Coéquipier 5'!D16,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="80"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7872,10 +7895,10 @@
         <f>VLOOKUP('Coéquipier 5'!D17,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7889,10 +7912,10 @@
         <f>VLOOKUP('Coéquipier 5'!D18,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="77"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7906,10 +7929,10 @@
         <f>VLOOKUP('Coéquipier 5'!D19,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="77"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7923,10 +7946,10 @@
         <f>VLOOKUP('Coéquipier 5'!D20,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F20" s="77"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="79"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7940,10 +7963,10 @@
         <f>VLOOKUP('Coéquipier 5'!D21,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="79"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7957,10 +7980,10 @@
         <f>VLOOKUP('Coéquipier 5'!D22,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7974,10 +7997,10 @@
         <f>VLOOKUP('Coéquipier 5'!D23,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F23" s="77"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="79"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="80"/>
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7991,10 +8014,10 @@
         <f>VLOOKUP('Coéquipier 5'!D24,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F24" s="77"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="79"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8008,10 +8031,10 @@
         <f>VLOOKUP('Coéquipier 5'!D25,Menu!$B$4:$C$8,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="82"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="83"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8026,12 +8049,12 @@
       <c r="C27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>